<commit_message>
Updated file locations of everything
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
@@ -505,25 +505,25 @@
         <v>72173</v>
       </c>
       <c r="F3" t="n">
-        <v>0.648291828587093</v>
+        <v>0.648290815188176</v>
       </c>
       <c r="G3" t="n">
-        <v>83960.4394621138</v>
+        <v>83960.4394597247</v>
       </c>
       <c r="H3" t="n">
-        <v>-167876.878924228</v>
+        <v>-167876.878919449</v>
       </c>
       <c r="I3" t="n">
-        <v>8720.75702850198</v>
+        <v>8720.7570332801</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-167674.768855766</v>
+        <v>-167674.768850988</v>
       </c>
       <c r="L3" t="n">
-        <v>32414.5685353517</v>
+        <v>32414.5685408552</v>
       </c>
       <c r="M3" t="n">
         <v>72151</v>

</xml_diff>

<commit_message>
Updated model model outputs for lmb and np
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
@@ -505,25 +505,25 @@
         <v>72173</v>
       </c>
       <c r="F3" t="n">
-        <v>0.648291274111411</v>
+        <v>0.648292676600048</v>
       </c>
       <c r="G3" t="n">
-        <v>83960.4394621176</v>
+        <v>83960.4394617256</v>
       </c>
       <c r="H3" t="n">
-        <v>-167876.878924235</v>
+        <v>-167876.878923451</v>
       </c>
       <c r="I3" t="n">
-        <v>8720.75702849432</v>
+        <v>8720.75702927841</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-167674.768855773</v>
+        <v>-167674.768854989</v>
       </c>
       <c r="L3" t="n">
-        <v>32414.5685427552</v>
+        <v>32414.5685920514</v>
       </c>
       <c r="M3" t="n">
         <v>72151</v>

</xml_diff>

<commit_message>
All results are updated
</commit_message>
<xml_diff>
--- a/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
+++ b/results/accel-glmm-results/glmm_model_selection_hab_season_np.xlsx
@@ -482,13 +482,13 @@
         <v>80579</v>
       </c>
       <c r="F2" t="n">
-        <v>0.10770847961907</v>
+        <v>0.10769139134775</v>
       </c>
       <c r="G2" t="n">
-        <v>97520.0880678259</v>
+        <v>97520.2281613775</v>
       </c>
       <c r="H2" t="n">
-        <v>-194874.176135652</v>
+        <v>-194874.456322755</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="n">
-        <v>-194102.525687715</v>
+        <v>-194102.805874818</v>
       </c>
       <c r="L2" t="n">
         <v>80496</v>
@@ -520,22 +520,22 @@
         <v>80579</v>
       </c>
       <c r="F3" t="n">
-        <v>0.108080375728955</v>
+        <v>0.108080375720078</v>
       </c>
       <c r="G3" t="n">
-        <v>96615.7110242614</v>
+        <v>96615.7110242586</v>
       </c>
       <c r="H3" t="n">
-        <v>-193195.422048523</v>
+        <v>-193195.422048517</v>
       </c>
       <c r="I3" t="n">
-        <v>1678.75408712894</v>
+        <v>1679.03427423778</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-193028.076168247</v>
+        <v>-193028.076168242</v>
       </c>
       <c r="L3" t="n">
         <v>80561</v>
@@ -558,22 +558,22 @@
         <v>80579</v>
       </c>
       <c r="F4" t="n">
-        <v>0.107710649480812</v>
+        <v>0.10771065056736</v>
       </c>
       <c r="G4" t="n">
-        <v>96249.9594431719</v>
+        <v>96249.9594431749</v>
       </c>
       <c r="H4" t="n">
-        <v>-192455.918886344</v>
+        <v>-192455.91888635</v>
       </c>
       <c r="I4" t="n">
-        <v>2418.25724930794</v>
+        <v>2418.53743640525</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>-192251.385032674</v>
+        <v>-192251.38503268</v>
       </c>
       <c r="L4" t="n">
         <v>80557</v>
@@ -596,22 +596,22 @@
         <v>80579</v>
       </c>
       <c r="F5" t="n">
-        <v>0.108351381263608</v>
+        <v>0.108351380927765</v>
       </c>
       <c r="G5" t="n">
-        <v>96220.8707511277</v>
+        <v>96220.8707511761</v>
       </c>
       <c r="H5" t="n">
-        <v>-192397.741502255</v>
+        <v>-192397.741502352</v>
       </c>
       <c r="I5" t="n">
-        <v>2476.43463339645</v>
+        <v>2476.71482040279</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-192193.207648585</v>
+        <v>-192193.207648682</v>
       </c>
       <c r="L5" t="n">
         <v>80557</v>
@@ -643,7 +643,7 @@
         <v>-192038.999911432</v>
       </c>
       <c r="I6" t="n">
-        <v>2835.17622421985</v>
+        <v>2835.4564113231</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -672,22 +672,22 @@
         <v>80579</v>
       </c>
       <c r="F7" t="n">
-        <v>0.108436433145196</v>
+        <v>0.108436433145375</v>
       </c>
       <c r="G7" t="n">
-        <v>95845.7489746321</v>
+        <v>95845.7489746352</v>
       </c>
       <c r="H7" t="n">
-        <v>-191679.497949264</v>
+        <v>-191679.49794927</v>
       </c>
       <c r="I7" t="n">
-        <v>3194.67818638749</v>
+        <v>3194.95837348461</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>-191623.715989172</v>
+        <v>-191623.715989179</v>
       </c>
       <c r="L7" t="n">
         <v>80573</v>
@@ -710,22 +710,22 @@
         <v>80579</v>
       </c>
       <c r="F8" t="n">
-        <v>0.108084000859689</v>
+        <v>0.108084000859814</v>
       </c>
       <c r="G8" t="n">
-        <v>95419.8018318779</v>
+        <v>95419.8018318762</v>
       </c>
       <c r="H8" t="n">
-        <v>-190825.603663756</v>
+        <v>-190825.603663752</v>
       </c>
       <c r="I8" t="n">
-        <v>4048.57247189604</v>
+        <v>4048.85265900267</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>-190760.524710315</v>
+        <v>-190760.524710312</v>
       </c>
       <c r="L8" t="n">
         <v>80572</v>

</xml_diff>